<commit_message>
desarrollo correspondiente al mantenedor de template, bloqueo de iniciativas, parametros comerciales y otros.
</commit_message>
<xml_diff>
--- a/Capex.Web/Capex.Web/Files/Downloads/TemplateExportExcelIniciativa.xlsx
+++ b/Capex.Web/Capex.Web/Files/Downloads/TemplateExportExcelIniciativa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enrique Cuevas\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37792038-EC5A-465F-B745-263C75E0BDF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8EAF9C-8EC3-4583-A53E-F8DA055C7AFD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F59F81DA-A5D5-40A9-AD26-6F2DBE826DA9}"/>
   </bookViews>
@@ -493,92 +493,92 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -997,7 +997,7 @@
   <dimension ref="B1:Z47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B23" sqref="B23:I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,159 +1023,159 @@
     <row r="1" spans="2:25" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="N3" s="43" t="s">
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="N3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="43"/>
-      <c r="P3" s="43"/>
-      <c r="Q3" s="43"/>
-      <c r="R3" s="43"/>
-      <c r="S3" s="43"/>
-      <c r="T3" s="43"/>
-      <c r="U3" s="43"/>
-      <c r="V3" s="43"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="27"/>
     </row>
     <row r="4" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="N4" s="43" t="s">
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="N4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="43"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="27"/>
     </row>
     <row r="5" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="35" t="s">
+      <c r="K7" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="44"/>
-      <c r="P7" s="44"/>
-      <c r="Q7" s="44"/>
-      <c r="R7" s="44"/>
-      <c r="S7" s="44"/>
-      <c r="T7" s="44"/>
-      <c r="U7" s="44"/>
-      <c r="V7" s="44"/>
-      <c r="W7" s="44"/>
-      <c r="X7" s="44"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+      <c r="W7" s="28"/>
+      <c r="X7" s="28"/>
     </row>
     <row r="8" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="35" t="s">
+      <c r="K8" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="44"/>
-      <c r="P8" s="44"/>
-      <c r="Q8" s="44"/>
-      <c r="R8" s="44"/>
-      <c r="S8" s="44"/>
-      <c r="T8" s="44"/>
-      <c r="U8" s="44"/>
-      <c r="V8" s="44"/>
-      <c r="W8" s="44"/>
-      <c r="X8" s="44"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="W8" s="28"/>
+      <c r="X8" s="28"/>
     </row>
     <row r="9" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="35" t="s">
+      <c r="K9" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="44"/>
-      <c r="R9" s="44"/>
-      <c r="S9" s="44"/>
-      <c r="T9" s="44"/>
-      <c r="U9" s="44"/>
-      <c r="V9" s="44"/>
-      <c r="W9" s="44"/>
-      <c r="X9" s="44"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
+      <c r="X9" s="28"/>
     </row>
     <row r="10" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="36"/>
+      <c r="G10" s="37"/>
       <c r="H10" s="4"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="30"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
-      <c r="S10" s="36" t="s">
+      <c r="S10" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="T10" s="36"/>
-      <c r="U10" s="36"/>
-      <c r="V10" s="32"/>
-      <c r="W10" s="32"/>
+      <c r="T10" s="37"/>
+      <c r="U10" s="37"/>
+      <c r="V10" s="29"/>
+      <c r="W10" s="29"/>
     </row>
     <row r="11" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
@@ -1201,12 +1201,12 @@
       <c r="U11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="V11" s="41"/>
-      <c r="W11" s="41"/>
-      <c r="X11" s="45" t="s">
+      <c r="V11" s="36"/>
+      <c r="W11" s="36"/>
+      <c r="X11" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="Y11" s="45"/>
+      <c r="Y11" s="31"/>
     </row>
     <row r="12" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
@@ -1235,32 +1235,32 @@
       <c r="H13" s="26"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="35" t="s">
+      <c r="K13" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="35"/>
-      <c r="U13" s="35"/>
-      <c r="V13" s="35"/>
-      <c r="W13" s="35"/>
-      <c r="X13" s="35"/>
-      <c r="Y13" s="35"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="33"/>
+      <c r="T13" s="33"/>
+      <c r="U13" s="33"/>
+      <c r="V13" s="33"/>
+      <c r="W13" s="33"/>
+      <c r="X13" s="33"/>
+      <c r="Y13" s="33"/>
     </row>
     <row r="14" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="7"/>
@@ -1308,13 +1308,13 @@
       </c>
     </row>
     <row r="15" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="10" t="s">
@@ -1374,13 +1374,13 @@
       <c r="Y16" s="7"/>
     </row>
     <row r="17" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="25"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="10" t="s">
@@ -1402,13 +1402,13 @@
       <c r="Y17" s="7"/>
     </row>
     <row r="18" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="12" t="s">
@@ -1430,8 +1430,8 @@
         <v>67</v>
       </c>
       <c r="S18" s="26"/>
-      <c r="T18" s="43"/>
-      <c r="U18" s="43"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="27"/>
     </row>
     <row r="19" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="26" t="s">
@@ -1452,122 +1452,122 @@
       <c r="K19" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="32"/>
-      <c r="R19" s="32"/>
-      <c r="S19" s="32"/>
-      <c r="T19" s="32"/>
-      <c r="U19" s="32"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+      <c r="T19" s="29"/>
+      <c r="U19" s="29"/>
     </row>
     <row r="20" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="32"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="32"/>
-      <c r="R20" s="32"/>
-      <c r="S20" s="32"/>
-      <c r="T20" s="32"/>
-      <c r="U20" s="32"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29"/>
+      <c r="T20" s="29"/>
+      <c r="U20" s="29"/>
     </row>
     <row r="21" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="32"/>
-      <c r="R21" s="32"/>
-      <c r="S21" s="32"/>
-      <c r="T21" s="32"/>
-      <c r="U21" s="32"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
+      <c r="T21" s="29"/>
+      <c r="U21" s="29"/>
     </row>
     <row r="22" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
       <c r="J22" s="3"/>
     </row>
     <row r="23" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="30" t="s">
+      <c r="K23" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="L23" s="30"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="30"/>
-      <c r="O23" s="30"/>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="30"/>
-      <c r="S23" s="30"/>
-      <c r="T23" s="30"/>
-      <c r="U23" s="30"/>
-      <c r="V23" s="30"/>
-      <c r="W23" s="30"/>
-      <c r="X23" s="30"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="25"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="25"/>
+      <c r="S23" s="25"/>
+      <c r="T23" s="25"/>
+      <c r="U23" s="25"/>
+      <c r="V23" s="25"/>
+      <c r="W23" s="25"/>
+      <c r="X23" s="25"/>
     </row>
     <row r="24" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
       <c r="J24" s="3"/>
-      <c r="K24" s="35" t="s">
+      <c r="K24" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="35"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
       <c r="P24" s="38"/>
       <c r="Q24" s="38"/>
       <c r="R24" s="26" t="s">
@@ -1581,14 +1581,14 @@
       <c r="X24" s="26"/>
     </row>
     <row r="25" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
       <c r="J25" s="3"/>
       <c r="K25" s="9" t="s">
         <v>57</v>
@@ -1605,50 +1605,50 @@
         <v>68</v>
       </c>
       <c r="Q25" s="26"/>
-      <c r="R25" s="39"/>
-      <c r="S25" s="39"/>
-      <c r="T25" s="39"/>
-      <c r="U25" s="39"/>
-      <c r="V25" s="39"/>
-      <c r="W25" s="39"/>
-      <c r="X25" s="39"/>
+      <c r="R25" s="35"/>
+      <c r="S25" s="35"/>
+      <c r="T25" s="35"/>
+      <c r="U25" s="35"/>
+      <c r="V25" s="35"/>
+      <c r="W25" s="35"/>
+      <c r="X25" s="35"/>
     </row>
     <row r="26" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
       <c r="J26" s="3"/>
       <c r="K26" s="14"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
-      <c r="O26" s="28"/>
-      <c r="P26" s="28"/>
-      <c r="Q26" s="28"/>
-      <c r="R26" s="39"/>
-      <c r="S26" s="39"/>
-      <c r="T26" s="39"/>
-      <c r="U26" s="39"/>
-      <c r="V26" s="39"/>
-      <c r="W26" s="39"/>
-      <c r="X26" s="39"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="34"/>
+      <c r="P26" s="34"/>
+      <c r="Q26" s="34"/>
+      <c r="R26" s="35"/>
+      <c r="S26" s="35"/>
+      <c r="T26" s="35"/>
+      <c r="U26" s="35"/>
+      <c r="V26" s="35"/>
+      <c r="W26" s="35"/>
+      <c r="X26" s="35"/>
     </row>
     <row r="27" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
       <c r="J27" s="3"/>
       <c r="K27" s="26" t="s">
         <v>56</v>
@@ -1659,23 +1659,23 @@
       <c r="O27" s="26"/>
       <c r="P27" s="38"/>
       <c r="Q27" s="38"/>
-      <c r="R27" s="39"/>
-      <c r="S27" s="39"/>
-      <c r="T27" s="39"/>
-      <c r="U27" s="39"/>
-      <c r="V27" s="39"/>
-      <c r="W27" s="39"/>
-      <c r="X27" s="39"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="35"/>
+      <c r="T27" s="35"/>
+      <c r="U27" s="35"/>
+      <c r="V27" s="35"/>
+      <c r="W27" s="35"/>
+      <c r="X27" s="35"/>
     </row>
     <row r="28" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
       <c r="J28" s="3"/>
       <c r="K28" s="9" t="s">
         <v>57</v>
@@ -1704,37 +1704,37 @@
       <c r="W28" s="26"/>
     </row>
     <row r="29" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
       <c r="J29" s="3"/>
       <c r="K29" s="14"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
-      <c r="O29" s="28"/>
-      <c r="P29" s="28"/>
-      <c r="Q29" s="28"/>
-      <c r="S29" s="42"/>
-      <c r="T29" s="42"/>
-      <c r="U29" s="42"/>
-      <c r="V29" s="42"/>
-      <c r="W29" s="42"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="34"/>
+      <c r="P29" s="34"/>
+      <c r="Q29" s="34"/>
+      <c r="S29" s="39"/>
+      <c r="T29" s="39"/>
+      <c r="U29" s="39"/>
+      <c r="V29" s="39"/>
+      <c r="W29" s="39"/>
     </row>
     <row r="30" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
@@ -1745,43 +1745,43 @@
       <c r="Q30" s="3"/>
     </row>
     <row r="31" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="30" t="s">
+      <c r="K31" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="L31" s="30"/>
-      <c r="M31" s="30"/>
-      <c r="N31" s="30"/>
-      <c r="O31" s="30"/>
-      <c r="P31" s="30"/>
-      <c r="Q31" s="30"/>
-      <c r="R31" s="30"/>
-      <c r="S31" s="30"/>
-      <c r="T31" s="30"/>
-      <c r="U31" s="30"/>
-      <c r="V31" s="30"/>
-      <c r="W31" s="30"/>
-      <c r="X31" s="30"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="25"/>
+      <c r="O31" s="25"/>
+      <c r="P31" s="25"/>
+      <c r="Q31" s="25"/>
+      <c r="R31" s="25"/>
+      <c r="S31" s="25"/>
+      <c r="T31" s="25"/>
+      <c r="U31" s="25"/>
+      <c r="V31" s="25"/>
+      <c r="W31" s="25"/>
+      <c r="X31" s="25"/>
     </row>
     <row r="32" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
       <c r="J32" s="3"/>
       <c r="K32" s="9" t="s">
         <v>69</v>
@@ -1802,81 +1802,81 @@
         <v>73</v>
       </c>
       <c r="S32" s="26"/>
-      <c r="T32" s="46"/>
-      <c r="U32" s="46"/>
+      <c r="T32" s="32"/>
+      <c r="U32" s="32"/>
     </row>
     <row r="33" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
       <c r="J33" s="3"/>
       <c r="K33" s="4"/>
-      <c r="L33" s="32"/>
-      <c r="M33" s="32"/>
-      <c r="N33" s="32"/>
-      <c r="O33" s="32"/>
-      <c r="P33" s="32"/>
-      <c r="Q33" s="32"/>
-      <c r="R33" s="40"/>
-      <c r="S33" s="40"/>
-      <c r="T33" s="32"/>
-      <c r="U33" s="32"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+      <c r="O33" s="29"/>
+      <c r="P33" s="29"/>
+      <c r="Q33" s="29"/>
+      <c r="R33" s="30"/>
+      <c r="S33" s="30"/>
+      <c r="T33" s="29"/>
+      <c r="U33" s="29"/>
     </row>
     <row r="34" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="33"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
       <c r="J34" s="3"/>
     </row>
     <row r="35" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="40"/>
       <c r="J35" s="3"/>
     </row>
     <row r="36" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
       <c r="J36" s="3"/>
-      <c r="K36" s="30" t="s">
+      <c r="K36" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="L36" s="30"/>
-      <c r="M36" s="30"/>
-      <c r="N36" s="30"/>
-      <c r="O36" s="30"/>
-      <c r="P36" s="30"/>
-      <c r="Q36" s="30"/>
-      <c r="R36" s="30"/>
-      <c r="S36" s="30"/>
-      <c r="T36" s="30"/>
-      <c r="U36" s="30"/>
-      <c r="V36" s="30"/>
-      <c r="W36" s="30"/>
-      <c r="X36" s="30"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="25"/>
+      <c r="P36" s="25"/>
+      <c r="Q36" s="25"/>
+      <c r="R36" s="25"/>
+      <c r="S36" s="25"/>
+      <c r="T36" s="25"/>
+      <c r="U36" s="25"/>
+      <c r="V36" s="25"/>
+      <c r="W36" s="25"/>
+      <c r="X36" s="25"/>
     </row>
     <row r="37" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="9" t="s">
@@ -1940,19 +1940,19 @@
       <c r="K38" s="24">
         <v>1</v>
       </c>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
-      <c r="O38" s="27"/>
-      <c r="P38" s="27"/>
-      <c r="Q38" s="28"/>
-      <c r="R38" s="28"/>
-      <c r="S38" s="28"/>
-      <c r="T38" s="28"/>
-      <c r="U38" s="28"/>
-      <c r="V38" s="28"/>
-      <c r="W38" s="28"/>
-      <c r="X38" s="28"/>
+      <c r="L38" s="45"/>
+      <c r="M38" s="45"/>
+      <c r="N38" s="45"/>
+      <c r="O38" s="45"/>
+      <c r="P38" s="45"/>
+      <c r="Q38" s="34"/>
+      <c r="R38" s="34"/>
+      <c r="S38" s="34"/>
+      <c r="T38" s="34"/>
+      <c r="U38" s="34"/>
+      <c r="V38" s="34"/>
+      <c r="W38" s="34"/>
+      <c r="X38" s="34"/>
     </row>
     <row r="39" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
@@ -1975,19 +1975,19 @@
       <c r="K39" s="24">
         <v>2</v>
       </c>
-      <c r="L39" s="27"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="27"/>
-      <c r="O39" s="27"/>
-      <c r="P39" s="27"/>
-      <c r="Q39" s="28"/>
-      <c r="R39" s="28"/>
-      <c r="S39" s="28"/>
-      <c r="T39" s="28"/>
-      <c r="U39" s="28"/>
-      <c r="V39" s="28"/>
-      <c r="W39" s="28"/>
-      <c r="X39" s="28"/>
+      <c r="L39" s="45"/>
+      <c r="M39" s="45"/>
+      <c r="N39" s="45"/>
+      <c r="O39" s="45"/>
+      <c r="P39" s="45"/>
+      <c r="Q39" s="34"/>
+      <c r="R39" s="34"/>
+      <c r="S39" s="34"/>
+      <c r="T39" s="34"/>
+      <c r="U39" s="34"/>
+      <c r="V39" s="34"/>
+      <c r="W39" s="34"/>
+      <c r="X39" s="34"/>
     </row>
     <row r="40" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="4"/>
@@ -2002,48 +2002,48 @@
       <c r="K40" s="24">
         <v>3</v>
       </c>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-      <c r="O40" s="27"/>
-      <c r="P40" s="27"/>
-      <c r="Q40" s="28"/>
-      <c r="R40" s="28"/>
-      <c r="S40" s="28"/>
-      <c r="T40" s="28"/>
-      <c r="U40" s="28"/>
-      <c r="V40" s="28"/>
-      <c r="W40" s="28"/>
-      <c r="X40" s="28"/>
+      <c r="L40" s="45"/>
+      <c r="M40" s="45"/>
+      <c r="N40" s="45"/>
+      <c r="O40" s="45"/>
+      <c r="P40" s="45"/>
+      <c r="Q40" s="34"/>
+      <c r="R40" s="34"/>
+      <c r="S40" s="34"/>
+      <c r="T40" s="34"/>
+      <c r="U40" s="34"/>
+      <c r="V40" s="34"/>
+      <c r="W40" s="34"/>
+      <c r="X40" s="34"/>
     </row>
     <row r="41" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C41" s="17"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="34"/>
-      <c r="I41" s="34"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
       <c r="J41" s="3"/>
-      <c r="K41" s="30" t="s">
+      <c r="K41" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="L41" s="30"/>
-      <c r="M41" s="30"/>
-      <c r="N41" s="30"/>
-      <c r="O41" s="30"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="30"/>
-      <c r="R41" s="30"/>
-      <c r="S41" s="30"/>
-      <c r="T41" s="30"/>
-      <c r="U41" s="30"/>
-      <c r="V41" s="30"/>
-      <c r="W41" s="30"/>
-      <c r="X41" s="30"/>
+      <c r="L41" s="25"/>
+      <c r="M41" s="25"/>
+      <c r="N41" s="25"/>
+      <c r="O41" s="25"/>
+      <c r="P41" s="25"/>
+      <c r="Q41" s="25"/>
+      <c r="R41" s="25"/>
+      <c r="S41" s="25"/>
+      <c r="T41" s="25"/>
+      <c r="U41" s="25"/>
+      <c r="V41" s="25"/>
+      <c r="W41" s="25"/>
+      <c r="X41" s="25"/>
     </row>
     <row r="42" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="26" t="s">
@@ -2079,14 +2079,14 @@
       <c r="X42" s="3"/>
     </row>
     <row r="43" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="28"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
-      <c r="I43" s="28"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34"/>
       <c r="J43" s="3"/>
       <c r="K43" s="19" t="s">
         <v>66</v>
@@ -2132,14 +2132,14 @@
       <c r="O44" s="22"/>
     </row>
     <row r="45" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
       <c r="J45" s="3"/>
       <c r="K45" s="19" t="s">
         <v>85</v>
@@ -2168,18 +2168,133 @@
       <c r="O46" s="22"/>
     </row>
     <row r="47" spans="2:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="H47" s="29" t="s">
+      <c r="H47" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="I47" s="29"/>
-      <c r="X47" s="29" t="s">
+      <c r="I47" s="46"/>
+      <c r="X47" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="Y47" s="29"/>
+      <c r="Y47" s="46"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="hT0R5dSroLLJ7JFp/gtcHUvOJIMoqKd4TE5v3481uknF/tixkdYB4wB4wtryhAJberR4fcqixo5ZOjUO6c4VxQ==" saltValue="uT1JGFtBJEH8pfs5FGnlVA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="136">
+  <sheetProtection password="D56A" sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="139">
+    <mergeCell ref="V37:X37"/>
+    <mergeCell ref="L40:P40"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="X47:Y47"/>
+    <mergeCell ref="K41:X41"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="S40:U40"/>
+    <mergeCell ref="V40:X40"/>
+    <mergeCell ref="L38:P38"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="S38:U38"/>
+    <mergeCell ref="V38:X38"/>
+    <mergeCell ref="L39:P39"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="S39:U39"/>
+    <mergeCell ref="V39:X39"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="P28:Q28"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="B33:I35"/>
+    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="D41:I41"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="K23:X23"/>
+    <mergeCell ref="K24:O24"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="E8:I8"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="K27:O27"/>
+    <mergeCell ref="P27:Q27"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="B20:C21"/>
+    <mergeCell ref="D20:E21"/>
+    <mergeCell ref="F20:H21"/>
+    <mergeCell ref="B14:C15"/>
+    <mergeCell ref="D14:E15"/>
+    <mergeCell ref="F14:H15"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B23:I26"/>
+    <mergeCell ref="B28:I31"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="P25:Q25"/>
+    <mergeCell ref="R25:X27"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="K13:Y13"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="S10:U10"/>
+    <mergeCell ref="R18:S18"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="R24:X24"/>
+    <mergeCell ref="U28:W28"/>
+    <mergeCell ref="U29:W29"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="T21:U21"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="N3:V3"/>
+    <mergeCell ref="N4:V4"/>
+    <mergeCell ref="O7:X7"/>
+    <mergeCell ref="O8:X8"/>
+    <mergeCell ref="P19:Q19"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="T19:U19"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K9:N9"/>
     <mergeCell ref="K36:X36"/>
     <mergeCell ref="L37:P37"/>
     <mergeCell ref="Q37:R37"/>
@@ -2204,118 +2319,6 @@
     <mergeCell ref="T20:U20"/>
     <mergeCell ref="L21:M21"/>
     <mergeCell ref="N21:O21"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="N3:V3"/>
-    <mergeCell ref="N4:V4"/>
-    <mergeCell ref="O7:X7"/>
-    <mergeCell ref="O8:X8"/>
-    <mergeCell ref="P19:Q19"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="T19:U19"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="P25:Q25"/>
-    <mergeCell ref="R25:X27"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="K13:Y13"/>
-    <mergeCell ref="V10:W10"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="R18:S18"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="R24:X24"/>
-    <mergeCell ref="U28:W28"/>
-    <mergeCell ref="U29:W29"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="S28:T28"/>
-    <mergeCell ref="S29:T29"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="T21:U21"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="B32:I32"/>
-    <mergeCell ref="B23:I26"/>
-    <mergeCell ref="B28:I31"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="E8:I8"/>
-    <mergeCell ref="E9:I9"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="K27:O27"/>
-    <mergeCell ref="P27:Q27"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="P28:Q28"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B33:I35"/>
-    <mergeCell ref="B36:I36"/>
-    <mergeCell ref="D41:I41"/>
-    <mergeCell ref="B27:I27"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="K23:X23"/>
-    <mergeCell ref="K24:O24"/>
-    <mergeCell ref="V37:X37"/>
-    <mergeCell ref="L40:P40"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="X47:Y47"/>
-    <mergeCell ref="K41:X41"/>
-    <mergeCell ref="Q40:R40"/>
-    <mergeCell ref="S40:U40"/>
-    <mergeCell ref="V40:X40"/>
-    <mergeCell ref="L38:P38"/>
-    <mergeCell ref="Q38:R38"/>
-    <mergeCell ref="S38:U38"/>
-    <mergeCell ref="V38:X38"/>
-    <mergeCell ref="L39:P39"/>
-    <mergeCell ref="Q39:R39"/>
-    <mergeCell ref="S39:U39"/>
-    <mergeCell ref="V39:X39"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>